<commit_message>
Pokracovat v razeni zakazniku pri vkladani do tabulky. Udelat jmena zakazniku na mape.
</commit_message>
<xml_diff>
--- a/Zakaznici.xlsx
+++ b/Zakaznici.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatka\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatka\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B35536-EF4B-438E-8535-EE26CCAF07D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A527637-7DE2-4E4A-8D2F-1BEC01BAD146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{36AC976F-F4C2-45FC-ABC8-2A6EF23E258F}"/>
+    <workbookView xWindow="12495" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{36AC976F-F4C2-45FC-ABC8-2A6EF23E258F}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -56,36 +56,6 @@
     <t>Pocet</t>
   </si>
   <si>
-    <t>Zakaznik_1</t>
-  </si>
-  <si>
-    <t>Zakaznik_2</t>
-  </si>
-  <si>
-    <t>Zakaznik_3</t>
-  </si>
-  <si>
-    <t>Zakaznik_4</t>
-  </si>
-  <si>
-    <t>Zakaznik_5</t>
-  </si>
-  <si>
-    <t>Zakaznik_6</t>
-  </si>
-  <si>
-    <t>Zakaznik_7</t>
-  </si>
-  <si>
-    <t>Zakaznik_8</t>
-  </si>
-  <si>
-    <t>Zakaznik_9</t>
-  </si>
-  <si>
-    <t>Zakaznik_10</t>
-  </si>
-  <si>
     <t>49.0624992</t>
   </si>
   <si>
@@ -144,6 +114,36 @@
   </si>
   <si>
     <t>16.2609167</t>
+  </si>
+  <si>
+    <t>Zakaznik_1_Rokytná</t>
+  </si>
+  <si>
+    <t>Zakaznik_2_Krumlov</t>
+  </si>
+  <si>
+    <t>Zakaznik_3_Polánka</t>
+  </si>
+  <si>
+    <t>Zakaznik_8_Krumlov_2</t>
+  </si>
+  <si>
+    <t>Zakaznik_7_Budkovice</t>
+  </si>
+  <si>
+    <t>Zakaznik_6_Letkovice</t>
+  </si>
+  <si>
+    <t>Zakaznik_5_Ivančice</t>
+  </si>
+  <si>
+    <t>Zakaznik_4_Dobřínsko</t>
+  </si>
+  <si>
+    <t>Zakaznik_10_Vémyslice</t>
+  </si>
+  <si>
+    <t>Zakaznik_9_Dobelice</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,13 +565,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
       <c r="D2" s="2">
         <v>0.25</v>
@@ -585,13 +585,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
       </c>
       <c r="D3" s="2">
         <v>0.125</v>
@@ -605,13 +605,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="2">
         <v>0.22916666666666666</v>
@@ -625,13 +625,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -645,13 +645,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -665,13 +665,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -685,13 +685,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -705,13 +705,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -725,13 +725,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -745,13 +745,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>

</xml_diff>